<commit_message>
New Components in the dashboard and changes in M2M
</commit_message>
<xml_diff>
--- a/server/client_data.xlsx
+++ b/server/client_data.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="26215"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tanooj/Downloads/dynamic_UI-prototype/server/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="24320" windowHeight="11480" activeTab="7"/>
+    <workbookView xWindow="240" yWindow="465" windowWidth="20730" windowHeight="11475" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Securities" sheetId="1" r:id="rId1"/>
@@ -21,7 +16,7 @@
     <sheet name="TopTradingStocks" sheetId="7" r:id="rId7"/>
     <sheet name="Pledged" sheetId="8" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="124519"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -843,8 +838,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -927,7 +922,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
@@ -956,7 +951,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
@@ -1019,7 +1013,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1054,7 +1048,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1262,38 +1256,38 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AB6"/>
   <sheetViews>
     <sheetView topLeftCell="T1" workbookViewId="0">
-      <selection activeCell="AD12" sqref="AD12"/>
+      <selection activeCell="Z3" sqref="Z3:Z6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="12" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4.6640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.83203125" style="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.83203125" style="7" customWidth="1"/>
-    <col min="5" max="5" width="13.6640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.5" style="7" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.33203125" style="7" bestFit="1" customWidth="1"/>
-    <col min="8" max="14" width="13.33203125" style="7" customWidth="1"/>
-    <col min="15" max="16" width="16.6640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="19.5" style="7" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="18.5" style="7" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="20.5" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.85546875" style="7" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="14" width="13.28515625" style="7" customWidth="1"/>
+    <col min="15" max="16" width="16.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="19.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="18.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="20.42578125" style="7" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="12" style="7" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="22.33203125" style="7" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="23.5" style="7" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="25.1640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="12.1640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="16.6640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="22.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="23.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="25.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="12.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="16.7109375" style="7" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="15" style="7" bestFit="1" customWidth="1"/>
-    <col min="27" max="16384" width="8.83203125" style="7"/>
+    <col min="27" max="16384" width="8.85546875" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:28" s="6" customFormat="1">
       <c r="A1" s="4" t="s">
         <v>37</v>
       </c>
@@ -1315,28 +1309,28 @@
       <c r="G1" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="H1" s="28" t="s">
+      <c r="H1" s="27" t="s">
         <v>210</v>
       </c>
-      <c r="I1" s="28" t="s">
+      <c r="I1" s="27" t="s">
         <v>216</v>
       </c>
-      <c r="J1" s="28" t="s">
+      <c r="J1" s="27" t="s">
         <v>217</v>
       </c>
-      <c r="K1" s="28" t="s">
+      <c r="K1" s="27" t="s">
         <v>215</v>
       </c>
-      <c r="L1" s="28" t="s">
+      <c r="L1" s="27" t="s">
         <v>214</v>
       </c>
-      <c r="M1" s="28" t="s">
+      <c r="M1" s="27" t="s">
         <v>213</v>
       </c>
-      <c r="N1" s="28" t="s">
+      <c r="N1" s="27" t="s">
         <v>212</v>
       </c>
-      <c r="O1" s="28" t="s">
+      <c r="O1" s="27" t="s">
         <v>211</v>
       </c>
       <c r="P1" s="8" t="s">
@@ -1375,11 +1369,11 @@
       <c r="AA1" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="AB1" s="30" t="s">
+      <c r="AB1" s="29" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="2" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:28" s="6" customFormat="1">
       <c r="A2" s="2" t="s">
         <v>49</v>
       </c>
@@ -1401,7 +1395,7 @@
       <c r="G2">
         <v>9821074160</v>
       </c>
-      <c r="H2" s="29" t="s">
+      <c r="H2" s="28" t="s">
         <v>222</v>
       </c>
       <c r="I2" t="s">
@@ -1456,7 +1450,7 @@
         <v>43831</v>
       </c>
       <c r="Z2" s="15">
-        <v>43862</v>
+        <v>43891</v>
       </c>
       <c r="AA2" s="5" t="s">
         <v>144</v>
@@ -1465,7 +1459,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:28">
       <c r="A3" s="7" t="s">
         <v>159</v>
       </c>
@@ -1487,7 +1481,7 @@
       <c r="G3">
         <v>9921055426</v>
       </c>
-      <c r="H3" s="29" t="s">
+      <c r="H3" s="28" t="s">
         <v>223</v>
       </c>
       <c r="I3" t="s">
@@ -1542,7 +1536,7 @@
         <v>43831</v>
       </c>
       <c r="Z3" s="15">
-        <v>43862</v>
+        <v>43891</v>
       </c>
       <c r="AA3" s="5" t="s">
         <v>144</v>
@@ -1551,7 +1545,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:28">
       <c r="A4" s="7" t="s">
         <v>181</v>
       </c>
@@ -1573,7 +1567,7 @@
       <c r="G4">
         <v>8477522264</v>
       </c>
-      <c r="H4" s="29" t="s">
+      <c r="H4" s="28" t="s">
         <v>224</v>
       </c>
       <c r="I4" t="s">
@@ -1628,7 +1622,7 @@
         <v>43831</v>
       </c>
       <c r="Z4" s="15">
-        <v>43862</v>
+        <v>43891</v>
       </c>
       <c r="AA4" s="5" t="s">
         <v>144</v>
@@ -1637,7 +1631,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:28">
       <c r="A5" s="14" t="s">
         <v>182</v>
       </c>
@@ -1659,7 +1653,7 @@
       <c r="G5">
         <v>9820565195</v>
       </c>
-      <c r="H5" s="29" t="s">
+      <c r="H5" s="28" t="s">
         <v>225</v>
       </c>
       <c r="I5" t="s">
@@ -1714,7 +1708,7 @@
         <v>43831</v>
       </c>
       <c r="Z5" s="15">
-        <v>43862</v>
+        <v>43891</v>
       </c>
       <c r="AA5" s="5" t="s">
         <v>144</v>
@@ -1723,7 +1717,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:28">
       <c r="A6" s="14" t="s">
         <v>158</v>
       </c>
@@ -1745,7 +1739,7 @@
       <c r="G6">
         <v>9973268525</v>
       </c>
-      <c r="H6" s="29" t="s">
+      <c r="H6" s="28" t="s">
         <v>226</v>
       </c>
       <c r="I6" t="s">
@@ -1800,7 +1794,7 @@
         <v>43831</v>
       </c>
       <c r="Z6" s="15">
-        <v>43862</v>
+        <v>43891</v>
       </c>
       <c r="AA6" s="5" t="s">
         <v>144</v>
@@ -1823,27 +1817,27 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H59"/>
   <sheetViews>
-    <sheetView topLeftCell="A53" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="11" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.5" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" style="7" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.5" style="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.6640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.5" style="7" customWidth="1"/>
-    <col min="7" max="7" width="14.1640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.33203125" style="7" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="8.83203125" style="7"/>
+    <col min="4" max="4" width="15.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.42578125" style="7" customWidth="1"/>
+    <col min="7" max="7" width="14.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="8.85546875" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" s="3" customFormat="1">
       <c r="A1" s="4" t="s">
         <v>45</v>
       </c>
@@ -1869,7 +1863,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8">
       <c r="A2" s="7">
         <v>1</v>
       </c>
@@ -1883,10 +1877,10 @@
         <v>258</v>
       </c>
       <c r="E2" s="13">
-        <v>43862</v>
+        <v>43891</v>
       </c>
       <c r="F2" s="7">
-        <v>6600</v>
+        <v>660</v>
       </c>
       <c r="G2" s="17">
         <v>50</v>
@@ -1895,7 +1889,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8">
       <c r="A3" s="7">
         <v>1</v>
       </c>
@@ -1909,19 +1903,19 @@
         <v>258</v>
       </c>
       <c r="E3" s="13">
-        <v>43863</v>
+        <v>43892</v>
       </c>
       <c r="F3" s="7">
-        <v>6520</v>
-      </c>
-      <c r="G3" s="27">
+        <v>652</v>
+      </c>
+      <c r="G3" s="26">
         <v>90</v>
       </c>
       <c r="H3" s="17" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8">
       <c r="A4" s="7">
         <v>1</v>
       </c>
@@ -1935,19 +1929,19 @@
         <v>258</v>
       </c>
       <c r="E4" s="13">
-        <v>43864</v>
+        <v>43893</v>
       </c>
       <c r="F4" s="7">
-        <v>7500</v>
-      </c>
-      <c r="G4" s="27">
+        <v>750</v>
+      </c>
+      <c r="G4" s="26">
         <v>72</v>
       </c>
       <c r="H4" s="17" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8">
       <c r="A5" s="7">
         <v>1</v>
       </c>
@@ -1961,19 +1955,19 @@
         <v>258</v>
       </c>
       <c r="E5" s="13">
-        <v>43865</v>
+        <v>43894</v>
       </c>
       <c r="F5" s="14">
-        <v>2300</v>
-      </c>
-      <c r="G5" s="27">
+        <v>230</v>
+      </c>
+      <c r="G5" s="26">
         <v>63</v>
       </c>
       <c r="H5" s="17" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8">
       <c r="A6" s="7">
         <v>1</v>
       </c>
@@ -1987,19 +1981,19 @@
         <v>258</v>
       </c>
       <c r="E6" s="13">
-        <v>43866</v>
+        <v>43895</v>
       </c>
       <c r="F6" s="14">
-        <v>1750</v>
-      </c>
-      <c r="G6" s="27">
+        <v>175</v>
+      </c>
+      <c r="G6" s="26">
         <v>105</v>
       </c>
       <c r="H6" s="17" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8">
       <c r="A7" s="7">
         <v>1</v>
       </c>
@@ -2013,19 +2007,19 @@
         <v>258</v>
       </c>
       <c r="E7" s="13">
-        <v>43867</v>
+        <v>43896</v>
       </c>
       <c r="F7" s="14">
-        <v>8000</v>
-      </c>
-      <c r="G7" s="27">
+        <v>800</v>
+      </c>
+      <c r="G7" s="26">
         <v>60</v>
       </c>
       <c r="H7" s="17" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8">
       <c r="A8" s="7">
         <v>1</v>
       </c>
@@ -2039,19 +2033,19 @@
         <v>258</v>
       </c>
       <c r="E8" s="13">
-        <v>43868</v>
+        <v>43897</v>
       </c>
       <c r="F8" s="14">
-        <v>4500</v>
-      </c>
-      <c r="G8" s="27">
+        <v>450</v>
+      </c>
+      <c r="G8" s="26">
         <v>30</v>
       </c>
       <c r="H8" s="17" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8">
       <c r="A9" s="7">
         <v>1</v>
       </c>
@@ -2065,19 +2059,19 @@
         <v>258</v>
       </c>
       <c r="E9" s="13">
-        <v>43869</v>
+        <v>43898</v>
       </c>
       <c r="F9" s="14">
-        <v>1800</v>
-      </c>
-      <c r="G9" s="27">
+        <v>180</v>
+      </c>
+      <c r="G9" s="26">
         <v>52</v>
       </c>
       <c r="H9" s="17" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8">
       <c r="A10" s="14">
         <v>2</v>
       </c>
@@ -2091,19 +2085,19 @@
         <v>259</v>
       </c>
       <c r="E10" s="25">
-        <v>43862</v>
+        <v>43891</v>
       </c>
       <c r="F10" s="14">
-        <v>14500</v>
-      </c>
-      <c r="G10" s="27">
+        <v>1450</v>
+      </c>
+      <c r="G10" s="26">
         <v>110</v>
       </c>
       <c r="H10" s="17" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8">
       <c r="A11" s="14">
         <v>2</v>
       </c>
@@ -2117,19 +2111,19 @@
         <v>259</v>
       </c>
       <c r="E11" s="25">
-        <v>43863</v>
+        <v>43892</v>
       </c>
       <c r="F11" s="14">
-        <v>12000</v>
-      </c>
-      <c r="G11" s="27">
+        <v>1200</v>
+      </c>
+      <c r="G11" s="26">
         <v>111</v>
       </c>
       <c r="H11" s="17" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8">
       <c r="A12" s="14">
         <v>2</v>
       </c>
@@ -2143,19 +2137,19 @@
         <v>259</v>
       </c>
       <c r="E12" s="25">
-        <v>43864</v>
+        <v>43893</v>
       </c>
       <c r="F12" s="14">
-        <v>25000</v>
-      </c>
-      <c r="G12" s="27">
+        <v>250</v>
+      </c>
+      <c r="G12" s="26">
         <v>20</v>
       </c>
       <c r="H12" s="17" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8">
       <c r="A13" s="14">
         <v>2</v>
       </c>
@@ -2169,19 +2163,19 @@
         <v>259</v>
       </c>
       <c r="E13" s="25">
-        <v>43865</v>
+        <v>43894</v>
       </c>
       <c r="F13" s="14">
-        <v>75000</v>
-      </c>
-      <c r="G13" s="27">
+        <v>750</v>
+      </c>
+      <c r="G13" s="26">
         <v>60</v>
       </c>
       <c r="H13" s="17" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8">
       <c r="A14" s="14">
         <v>2</v>
       </c>
@@ -2195,19 +2189,19 @@
         <v>259</v>
       </c>
       <c r="E14" s="25">
-        <v>43866</v>
+        <v>43895</v>
       </c>
       <c r="F14" s="14">
-        <v>65000</v>
-      </c>
-      <c r="G14" s="27">
+        <v>650</v>
+      </c>
+      <c r="G14" s="26">
         <v>40</v>
       </c>
       <c r="H14" s="17" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8">
       <c r="A15" s="14">
         <v>2</v>
       </c>
@@ -2221,19 +2215,19 @@
         <v>259</v>
       </c>
       <c r="E15" s="25">
-        <v>43867</v>
+        <v>43896</v>
       </c>
       <c r="F15" s="14">
-        <v>12000</v>
-      </c>
-      <c r="G15" s="27">
+        <v>120</v>
+      </c>
+      <c r="G15" s="26">
         <v>49</v>
       </c>
       <c r="H15" s="17" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8">
       <c r="A16" s="14">
         <v>2</v>
       </c>
@@ -2247,19 +2241,19 @@
         <v>259</v>
       </c>
       <c r="E16" s="25">
-        <v>43868</v>
+        <v>43897</v>
       </c>
       <c r="F16" s="14">
-        <v>165000</v>
-      </c>
-      <c r="G16" s="27">
+        <v>1650</v>
+      </c>
+      <c r="G16" s="26">
         <v>115</v>
       </c>
       <c r="H16" s="17" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8">
       <c r="A17" s="14">
         <v>2</v>
       </c>
@@ -2273,19 +2267,19 @@
         <v>259</v>
       </c>
       <c r="E17" s="25">
-        <v>43869</v>
+        <v>43898</v>
       </c>
       <c r="F17" s="14">
-        <v>85000</v>
-      </c>
-      <c r="G17" s="27">
+        <v>850</v>
+      </c>
+      <c r="G17" s="26">
         <v>20</v>
       </c>
       <c r="H17" s="17" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8">
       <c r="A18" s="14">
         <v>2</v>
       </c>
@@ -2299,19 +2293,19 @@
         <v>259</v>
       </c>
       <c r="E18" s="25">
-        <v>43870</v>
+        <v>43899</v>
       </c>
       <c r="F18" s="14">
-        <v>67520</v>
-      </c>
-      <c r="G18" s="27">
+        <v>675</v>
+      </c>
+      <c r="G18" s="26">
         <v>69</v>
       </c>
       <c r="H18" s="17" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8">
       <c r="A19" s="14">
         <v>2</v>
       </c>
@@ -2325,19 +2319,19 @@
         <v>259</v>
       </c>
       <c r="E19" s="25">
-        <v>43871</v>
+        <v>43900</v>
       </c>
       <c r="F19" s="14">
-        <v>18900</v>
-      </c>
-      <c r="G19" s="27">
+        <v>189</v>
+      </c>
+      <c r="G19" s="26">
         <v>32</v>
       </c>
       <c r="H19" s="17" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8">
       <c r="A20" s="14">
         <v>3</v>
       </c>
@@ -2351,19 +2345,19 @@
         <v>260</v>
       </c>
       <c r="E20" s="25">
-        <v>43862</v>
+        <v>43891</v>
       </c>
       <c r="F20" s="14">
         <v>400</v>
       </c>
-      <c r="G20" s="27">
+      <c r="G20" s="26">
         <v>28</v>
       </c>
       <c r="H20" s="17" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8">
       <c r="A21" s="14">
         <v>3</v>
       </c>
@@ -2377,19 +2371,19 @@
         <v>260</v>
       </c>
       <c r="E21" s="25">
-        <v>43863</v>
+        <v>43892</v>
       </c>
       <c r="F21" s="14">
-        <v>5000</v>
-      </c>
-      <c r="G21" s="27">
+        <v>500</v>
+      </c>
+      <c r="G21" s="26">
         <v>49</v>
       </c>
       <c r="H21" s="17" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8">
       <c r="A22" s="14">
         <v>3</v>
       </c>
@@ -2403,19 +2397,19 @@
         <v>260</v>
       </c>
       <c r="E22" s="25">
-        <v>43864</v>
+        <v>43893</v>
       </c>
       <c r="F22" s="14">
-        <v>8900</v>
-      </c>
-      <c r="G22" s="27">
+        <v>890</v>
+      </c>
+      <c r="G22" s="26">
         <v>36</v>
       </c>
       <c r="H22" s="17" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8">
       <c r="A23" s="14">
         <v>3</v>
       </c>
@@ -2429,19 +2423,19 @@
         <v>260</v>
       </c>
       <c r="E23" s="25">
-        <v>43865</v>
+        <v>43894</v>
       </c>
       <c r="F23" s="14">
-        <v>1400</v>
-      </c>
-      <c r="G23" s="27">
+        <v>140</v>
+      </c>
+      <c r="G23" s="26">
         <v>20</v>
       </c>
       <c r="H23" s="17" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8">
       <c r="A24" s="14">
         <v>3</v>
       </c>
@@ -2455,19 +2449,19 @@
         <v>260</v>
       </c>
       <c r="E24" s="25">
-        <v>43866</v>
+        <v>43895</v>
       </c>
       <c r="F24" s="14">
-        <v>15000</v>
-      </c>
-      <c r="G24" s="27">
+        <v>150</v>
+      </c>
+      <c r="G24" s="26">
         <v>120</v>
       </c>
       <c r="H24" s="17" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8">
       <c r="A25" s="14">
         <v>3</v>
       </c>
@@ -2481,19 +2475,19 @@
         <v>260</v>
       </c>
       <c r="E25" s="25">
-        <v>43867</v>
+        <v>43896</v>
       </c>
       <c r="F25" s="14">
         <v>1650</v>
       </c>
-      <c r="G25" s="27">
+      <c r="G25" s="26">
         <v>36</v>
       </c>
       <c r="H25" s="17" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8">
       <c r="A26" s="14">
         <v>3</v>
       </c>
@@ -2507,19 +2501,19 @@
         <v>260</v>
       </c>
       <c r="E26" s="25">
-        <v>43868</v>
+        <v>43897</v>
       </c>
       <c r="F26" s="14">
-        <v>43000</v>
-      </c>
-      <c r="G26" s="27">
+        <v>430</v>
+      </c>
+      <c r="G26" s="26">
         <v>94</v>
       </c>
       <c r="H26" s="17" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8">
       <c r="A27" s="14">
         <v>3</v>
       </c>
@@ -2533,19 +2527,19 @@
         <v>260</v>
       </c>
       <c r="E27" s="25">
-        <v>43869</v>
+        <v>43898</v>
       </c>
       <c r="F27" s="14">
-        <v>8900</v>
-      </c>
-      <c r="G27" s="27">
+        <v>890</v>
+      </c>
+      <c r="G27" s="26">
         <v>87</v>
       </c>
       <c r="H27" s="17" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:8">
       <c r="A28" s="14">
         <v>3</v>
       </c>
@@ -2559,19 +2553,19 @@
         <v>260</v>
       </c>
       <c r="E28" s="25">
-        <v>43870</v>
+        <v>43899</v>
       </c>
       <c r="F28" s="14">
-        <v>65000</v>
-      </c>
-      <c r="G28" s="27">
+        <v>650</v>
+      </c>
+      <c r="G28" s="26">
         <v>52</v>
       </c>
       <c r="H28" s="17" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:8">
       <c r="A29" s="14">
         <v>3</v>
       </c>
@@ -2585,19 +2579,19 @@
         <v>260</v>
       </c>
       <c r="E29" s="25">
-        <v>43871</v>
+        <v>43900</v>
       </c>
       <c r="F29" s="14">
-        <v>14789</v>
-      </c>
-      <c r="G29" s="27">
+        <v>1479</v>
+      </c>
+      <c r="G29" s="26">
         <v>62</v>
       </c>
       <c r="H29" s="17" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:8">
       <c r="A30" s="14">
         <v>4</v>
       </c>
@@ -2611,19 +2605,19 @@
         <v>261</v>
       </c>
       <c r="E30" s="25">
-        <v>43862</v>
+        <v>43891</v>
       </c>
       <c r="F30" s="14">
-        <v>150000</v>
-      </c>
-      <c r="G30" s="27">
+        <v>1500</v>
+      </c>
+      <c r="G30" s="26">
         <v>40</v>
       </c>
       <c r="H30" s="17" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:8">
       <c r="A31" s="14">
         <v>4</v>
       </c>
@@ -2637,19 +2631,19 @@
         <v>261</v>
       </c>
       <c r="E31" s="25">
-        <v>43863</v>
+        <v>43892</v>
       </c>
       <c r="F31" s="14">
-        <v>175000</v>
-      </c>
-      <c r="G31" s="27">
+        <v>1750</v>
+      </c>
+      <c r="G31" s="26">
         <v>103</v>
       </c>
       <c r="H31" s="17" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:8">
       <c r="A32" s="14">
         <v>4</v>
       </c>
@@ -2663,19 +2657,19 @@
         <v>261</v>
       </c>
       <c r="E32" s="25">
-        <v>43864</v>
+        <v>43893</v>
       </c>
       <c r="F32" s="14">
-        <v>250000</v>
-      </c>
-      <c r="G32" s="27">
+        <v>250</v>
+      </c>
+      <c r="G32" s="26">
         <v>60</v>
       </c>
       <c r="H32" s="17" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:8">
       <c r="A33" s="14">
         <v>4</v>
       </c>
@@ -2689,19 +2683,19 @@
         <v>261</v>
       </c>
       <c r="E33" s="25">
-        <v>43865</v>
+        <v>43894</v>
       </c>
       <c r="F33" s="14">
-        <v>125000</v>
-      </c>
-      <c r="G33" s="27">
+        <v>1250</v>
+      </c>
+      <c r="G33" s="26">
         <v>50</v>
       </c>
       <c r="H33" s="17" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:8">
       <c r="A34" s="14">
         <v>4</v>
       </c>
@@ -2715,19 +2709,19 @@
         <v>261</v>
       </c>
       <c r="E34" s="25">
-        <v>43866</v>
+        <v>43895</v>
       </c>
       <c r="F34" s="14">
-        <v>100000</v>
-      </c>
-      <c r="G34" s="27">
+        <v>100</v>
+      </c>
+      <c r="G34" s="26">
         <v>57</v>
       </c>
       <c r="H34" s="17" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:8">
       <c r="A35" s="14">
         <v>4</v>
       </c>
@@ -2741,19 +2735,19 @@
         <v>261</v>
       </c>
       <c r="E35" s="25">
-        <v>43867</v>
+        <v>43896</v>
       </c>
       <c r="F35" s="14">
-        <v>165000</v>
-      </c>
-      <c r="G35" s="27">
+        <v>165</v>
+      </c>
+      <c r="G35" s="26">
         <v>80</v>
       </c>
       <c r="H35" s="17" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:8">
       <c r="A36" s="14">
         <v>4</v>
       </c>
@@ -2767,19 +2761,19 @@
         <v>261</v>
       </c>
       <c r="E36" s="25">
-        <v>43868</v>
+        <v>43897</v>
       </c>
       <c r="F36" s="14">
-        <v>4500</v>
-      </c>
-      <c r="G36" s="27">
+        <v>450</v>
+      </c>
+      <c r="G36" s="26">
         <v>39</v>
       </c>
       <c r="H36" s="17" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:8">
       <c r="A37" s="14">
         <v>4</v>
       </c>
@@ -2793,19 +2787,19 @@
         <v>261</v>
       </c>
       <c r="E37" s="25">
-        <v>43869</v>
+        <v>43898</v>
       </c>
       <c r="F37" s="14">
-        <v>69450</v>
-      </c>
-      <c r="G37" s="27">
+        <v>694</v>
+      </c>
+      <c r="G37" s="26">
         <v>40</v>
       </c>
       <c r="H37" s="17" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:8">
       <c r="A38" s="14">
         <v>4</v>
       </c>
@@ -2819,19 +2813,19 @@
         <v>261</v>
       </c>
       <c r="E38" s="25">
-        <v>43870</v>
+        <v>43899</v>
       </c>
       <c r="F38" s="14">
         <v>456</v>
       </c>
-      <c r="G38" s="27">
+      <c r="G38" s="26">
         <v>5</v>
       </c>
       <c r="H38" s="17" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:8">
       <c r="A39" s="14">
         <v>4</v>
       </c>
@@ -2845,19 +2839,19 @@
         <v>261</v>
       </c>
       <c r="E39" s="25">
-        <v>43871</v>
+        <v>43900</v>
       </c>
       <c r="F39" s="14">
         <v>25</v>
       </c>
-      <c r="G39" s="27">
+      <c r="G39" s="26">
         <v>105</v>
       </c>
       <c r="H39" s="17" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:8">
       <c r="A40" s="14">
         <v>4</v>
       </c>
@@ -2871,19 +2865,19 @@
         <v>261</v>
       </c>
       <c r="E40" s="25">
-        <v>43872</v>
+        <v>43901</v>
       </c>
       <c r="F40" s="14">
-        <v>1489654</v>
-      </c>
-      <c r="G40" s="27">
+        <v>148</v>
+      </c>
+      <c r="G40" s="26">
         <v>60</v>
       </c>
       <c r="H40" s="17" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:8">
       <c r="A41" s="14">
         <v>4</v>
       </c>
@@ -2897,19 +2891,19 @@
         <v>261</v>
       </c>
       <c r="E41" s="25">
-        <v>43873</v>
+        <v>43902</v>
       </c>
       <c r="F41" s="14">
         <v>155</v>
       </c>
-      <c r="G41" s="27">
+      <c r="G41" s="26">
         <v>70</v>
       </c>
       <c r="H41" s="17" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:8">
       <c r="A42" s="14">
         <v>4</v>
       </c>
@@ -2923,19 +2917,19 @@
         <v>261</v>
       </c>
       <c r="E42" s="25">
-        <v>43874</v>
+        <v>43903</v>
       </c>
       <c r="F42" s="14">
-        <v>214544</v>
-      </c>
-      <c r="G42" s="27">
+        <v>214</v>
+      </c>
+      <c r="G42" s="26">
         <v>45</v>
       </c>
       <c r="H42" s="17" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:8">
       <c r="A43" s="14">
         <v>5</v>
       </c>
@@ -2949,19 +2943,19 @@
         <v>262</v>
       </c>
       <c r="E43" s="25">
-        <v>43862</v>
+        <v>43891</v>
       </c>
       <c r="F43" s="14">
-        <v>75000</v>
-      </c>
-      <c r="G43" s="27">
+        <v>750</v>
+      </c>
+      <c r="G43" s="26">
         <v>50</v>
       </c>
       <c r="H43" s="17" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:8">
       <c r="A44" s="14">
         <v>5</v>
       </c>
@@ -2975,19 +2969,19 @@
         <v>262</v>
       </c>
       <c r="E44" s="25">
-        <v>43863</v>
+        <v>43892</v>
       </c>
       <c r="F44" s="14">
-        <v>65000</v>
-      </c>
-      <c r="G44" s="27">
+        <v>650</v>
+      </c>
+      <c r="G44" s="26">
         <v>110</v>
       </c>
       <c r="H44" s="17" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:8">
       <c r="A45" s="14">
         <v>5</v>
       </c>
@@ -3001,19 +2995,19 @@
         <v>262</v>
       </c>
       <c r="E45" s="25">
-        <v>43864</v>
+        <v>43893</v>
       </c>
       <c r="F45" s="14">
-        <v>12000</v>
-      </c>
-      <c r="G45" s="27">
+        <v>120</v>
+      </c>
+      <c r="G45" s="26">
         <v>110</v>
       </c>
       <c r="H45" s="17" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:8">
       <c r="A46" s="14">
         <v>5</v>
       </c>
@@ -3027,19 +3021,19 @@
         <v>262</v>
       </c>
       <c r="E46" s="25">
-        <v>43865</v>
+        <v>43894</v>
       </c>
       <c r="F46" s="14">
-        <v>165000</v>
-      </c>
-      <c r="G46" s="27">
+        <v>1650</v>
+      </c>
+      <c r="G46" s="26">
         <v>60</v>
       </c>
       <c r="H46" s="17" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:8">
       <c r="A47" s="14">
         <v>5</v>
       </c>
@@ -3053,19 +3047,19 @@
         <v>262</v>
       </c>
       <c r="E47" s="25">
-        <v>43866</v>
+        <v>43895</v>
       </c>
       <c r="F47" s="14">
-        <v>85000</v>
-      </c>
-      <c r="G47" s="27">
+        <v>850</v>
+      </c>
+      <c r="G47" s="26">
         <v>50</v>
       </c>
       <c r="H47" s="17" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:8">
       <c r="A48" s="14">
         <v>5</v>
       </c>
@@ -3079,19 +3073,19 @@
         <v>262</v>
       </c>
       <c r="E48" s="25">
-        <v>43867</v>
+        <v>43896</v>
       </c>
       <c r="F48" s="14">
-        <v>67520</v>
-      </c>
-      <c r="G48" s="27">
+        <v>675</v>
+      </c>
+      <c r="G48" s="26">
         <v>40</v>
       </c>
       <c r="H48" s="17" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:8">
       <c r="A49" s="14">
         <v>5</v>
       </c>
@@ -3105,19 +3099,19 @@
         <v>262</v>
       </c>
       <c r="E49" s="25">
-        <v>43868</v>
+        <v>43897</v>
       </c>
       <c r="F49" s="14">
-        <v>18900</v>
-      </c>
-      <c r="G49" s="27">
+        <v>1890</v>
+      </c>
+      <c r="G49" s="26">
         <v>70</v>
       </c>
       <c r="H49" s="17" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:8">
       <c r="A50" s="14">
         <v>5</v>
       </c>
@@ -3131,19 +3125,19 @@
         <v>262</v>
       </c>
       <c r="E50" s="25">
-        <v>43869</v>
+        <v>43898</v>
       </c>
       <c r="F50" s="14">
         <v>400</v>
       </c>
-      <c r="G50" s="27">
+      <c r="G50" s="26">
         <v>80</v>
       </c>
       <c r="H50" s="17" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:8">
       <c r="A51" s="14">
         <v>5</v>
       </c>
@@ -3157,19 +3151,19 @@
         <v>262</v>
       </c>
       <c r="E51" s="25">
-        <v>43870</v>
+        <v>43899</v>
       </c>
       <c r="F51" s="14">
-        <v>5000</v>
-      </c>
-      <c r="G51" s="27">
+        <v>500</v>
+      </c>
+      <c r="G51" s="26">
         <v>90</v>
       </c>
       <c r="H51" s="17" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:8">
       <c r="A52" s="14">
         <v>5</v>
       </c>
@@ -3183,19 +3177,19 @@
         <v>262</v>
       </c>
       <c r="E52" s="25">
-        <v>43871</v>
+        <v>43900</v>
       </c>
       <c r="F52" s="14">
-        <v>8900</v>
-      </c>
-      <c r="G52" s="27">
+        <v>890</v>
+      </c>
+      <c r="G52" s="26">
         <v>50</v>
       </c>
       <c r="H52" s="17" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:8">
       <c r="A53" s="14">
         <v>5</v>
       </c>
@@ -3209,19 +3203,19 @@
         <v>262</v>
       </c>
       <c r="E53" s="25">
-        <v>43872</v>
+        <v>43901</v>
       </c>
       <c r="F53" s="14">
-        <v>1400</v>
-      </c>
-      <c r="G53" s="27">
+        <v>140</v>
+      </c>
+      <c r="G53" s="26">
         <v>40</v>
       </c>
       <c r="H53" s="17" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:8">
       <c r="A54" s="14">
         <v>5</v>
       </c>
@@ -3235,19 +3229,19 @@
         <v>262</v>
       </c>
       <c r="E54" s="25">
-        <v>43873</v>
+        <v>43902</v>
       </c>
       <c r="F54" s="14">
-        <v>15000</v>
-      </c>
-      <c r="G54" s="27">
+        <v>150</v>
+      </c>
+      <c r="G54" s="26">
         <v>70</v>
       </c>
       <c r="H54" s="17" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:8">
       <c r="A55" s="14">
         <v>5</v>
       </c>
@@ -3261,28 +3255,28 @@
         <v>262</v>
       </c>
       <c r="E55" s="25">
-        <v>43874</v>
+        <v>43903</v>
       </c>
       <c r="F55" s="14">
         <v>1650</v>
       </c>
-      <c r="G55" s="27">
+      <c r="G55" s="26">
         <v>50</v>
       </c>
       <c r="H55" s="17" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:8">
       <c r="F56" s="14"/>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:8">
       <c r="F57" s="14"/>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:8">
       <c r="F58" s="14"/>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:8">
       <c r="F59" s="14"/>
     </row>
   </sheetData>
@@ -3292,16 +3286,16 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:BS1"/>
   <sheetViews>
     <sheetView topLeftCell="BN1" workbookViewId="0">
-      <selection activeCell="BW1" sqref="BW1"/>
+      <selection activeCell="BQ26" sqref="BQ26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:71" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:71">
       <c r="A1" t="s">
         <v>52</v>
       </c>
@@ -3498,54 +3492,54 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AJ6"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.33203125" customWidth="1"/>
-    <col min="10" max="10" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.5" customWidth="1"/>
-    <col min="13" max="13" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="17.83203125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="4.5" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.28515625" customWidth="1"/>
+    <col min="10" max="10" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.42578125" customWidth="1"/>
+    <col min="13" max="13" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="12" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="20.7109375" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="20" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="9.1640625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="7.6640625" customWidth="1"/>
-    <col min="36" max="36" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="7.7109375" customWidth="1"/>
+    <col min="36" max="36" width="8.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:36">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -3655,7 +3649,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:36">
       <c r="A2" t="s">
         <v>113</v>
       </c>
@@ -3719,7 +3713,7 @@
       <c r="U2" t="s">
         <v>121</v>
       </c>
-      <c r="V2" s="29" t="s">
+      <c r="V2" s="28" t="s">
         <v>245</v>
       </c>
       <c r="W2" t="s">
@@ -3765,7 +3759,7 @@
         <v>43833</v>
       </c>
     </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:36">
       <c r="A3" t="s">
         <v>113</v>
       </c>
@@ -3829,7 +3823,7 @@
       <c r="U3" t="s">
         <v>241</v>
       </c>
-      <c r="V3" s="29" t="s">
+      <c r="V3" s="28" t="s">
         <v>246</v>
       </c>
       <c r="W3" t="s">
@@ -3875,7 +3869,7 @@
         <v>43833</v>
       </c>
     </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:36">
       <c r="A4" t="s">
         <v>113</v>
       </c>
@@ -3939,7 +3933,7 @@
       <c r="U4" t="s">
         <v>242</v>
       </c>
-      <c r="V4" s="29" t="s">
+      <c r="V4" s="28" t="s">
         <v>247</v>
       </c>
       <c r="W4" t="s">
@@ -3985,7 +3979,7 @@
         <v>43833</v>
       </c>
     </row>
-    <row r="5" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:36">
       <c r="A5" t="s">
         <v>113</v>
       </c>
@@ -4049,7 +4043,7 @@
       <c r="U5" t="s">
         <v>243</v>
       </c>
-      <c r="V5" s="29" t="s">
+      <c r="V5" s="28" t="s">
         <v>248</v>
       </c>
       <c r="W5" t="s">
@@ -4095,7 +4089,7 @@
         <v>43833</v>
       </c>
     </row>
-    <row r="6" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:36">
       <c r="A6" t="s">
         <v>113</v>
       </c>
@@ -4159,7 +4153,7 @@
       <c r="U6" t="s">
         <v>244</v>
       </c>
-      <c r="V6" s="29" t="s">
+      <c r="V6" s="28" t="s">
         <v>177</v>
       </c>
       <c r="W6" t="s">
@@ -4211,32 +4205,32 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.33203125" customWidth="1"/>
-    <col min="4" max="4" width="10.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" customWidth="1"/>
+    <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.1640625" customWidth="1"/>
-    <col min="8" max="8" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="21.5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="21.5" customWidth="1"/>
-    <col min="13" max="13" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.140625" customWidth="1"/>
+    <col min="8" max="8" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21.42578125" customWidth="1"/>
+    <col min="13" max="13" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -4280,7 +4274,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14">
       <c r="A2" s="16">
         <v>43831</v>
       </c>
@@ -4326,7 +4320,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14">
       <c r="A3" s="16">
         <v>43832</v>
       </c>
@@ -4372,7 +4366,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14">
       <c r="A4" s="16">
         <v>43833</v>
       </c>
@@ -4418,7 +4412,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14">
       <c r="A5" s="16">
         <v>43831</v>
       </c>
@@ -4464,7 +4458,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14">
       <c r="A6" s="16">
         <v>43832</v>
       </c>
@@ -4510,7 +4504,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14">
       <c r="A7" s="16">
         <v>43831</v>
       </c>
@@ -4556,7 +4550,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14">
       <c r="A8" s="16">
         <v>43832</v>
       </c>
@@ -4602,7 +4596,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14">
       <c r="A9" s="16">
         <v>43834</v>
       </c>
@@ -4648,7 +4642,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14">
       <c r="A10" s="16">
         <v>43835</v>
       </c>
@@ -4694,7 +4688,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14">
       <c r="A11" s="16">
         <v>43832</v>
       </c>
@@ -4740,7 +4734,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14">
       <c r="A12" s="16">
         <v>43833</v>
       </c>
@@ -4786,7 +4780,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14">
       <c r="A13" s="16">
         <v>43831</v>
       </c>
@@ -4832,7 +4826,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:14">
       <c r="A14" s="16">
         <v>43832</v>
       </c>
@@ -4878,7 +4872,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:14">
       <c r="A15" s="16">
         <v>43837</v>
       </c>
@@ -4924,7 +4918,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14">
       <c r="A16" s="16">
         <v>43836</v>
       </c>
@@ -4977,30 +4971,30 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="S26" sqref="S26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="17.6640625" customWidth="1"/>
-    <col min="2" max="2" width="10.1640625" customWidth="1"/>
-    <col min="3" max="3" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.33203125" customWidth="1"/>
-    <col min="5" max="5" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.7109375" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" customWidth="1"/>
+    <col min="3" max="3" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.28515625" customWidth="1"/>
+    <col min="5" max="5" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="23" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14">
       <c r="A1" t="s">
         <v>34</v>
       </c>
@@ -5044,7 +5038,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14">
       <c r="A2" s="2" t="s">
         <v>50</v>
       </c>
@@ -5094,21 +5088,21 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+      <selection activeCell="B18" sqref="B18:B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="11" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="11" width="13.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11">
       <c r="A1" t="s">
         <v>37</v>
       </c>
@@ -5143,12 +5137,12 @@
         <v>201</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11">
       <c r="A2" t="s">
         <v>49</v>
       </c>
       <c r="B2" s="22">
-        <v>43862</v>
+        <v>43891</v>
       </c>
       <c r="C2" s="19" t="s">
         <v>203</v>
@@ -5178,12 +5172,12 @@
         <v>450</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11">
       <c r="A3" t="s">
         <v>49</v>
       </c>
       <c r="B3" s="22">
-        <v>43863</v>
+        <v>43892</v>
       </c>
       <c r="C3" s="19" t="s">
         <v>203</v>
@@ -5213,12 +5207,12 @@
         <v>890</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11">
       <c r="A4" t="s">
         <v>49</v>
       </c>
       <c r="B4" s="22">
-        <v>43864</v>
+        <v>43893</v>
       </c>
       <c r="C4" s="19" t="s">
         <v>203</v>
@@ -5248,12 +5242,12 @@
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11">
       <c r="A5" t="s">
         <v>49</v>
       </c>
       <c r="B5" s="22">
-        <v>43865</v>
+        <v>43894</v>
       </c>
       <c r="C5" s="19" t="s">
         <v>203</v>
@@ -5283,12 +5277,12 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11">
       <c r="A6" t="s">
         <v>159</v>
       </c>
       <c r="B6" s="22">
-        <v>43862</v>
+        <v>43891</v>
       </c>
       <c r="C6" s="19" t="s">
         <v>163</v>
@@ -5318,12 +5312,12 @@
         <v>100</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11">
       <c r="A7" t="s">
         <v>159</v>
       </c>
       <c r="B7" s="22">
-        <v>43863</v>
+        <v>43892</v>
       </c>
       <c r="C7" s="19" t="s">
         <v>163</v>
@@ -5353,12 +5347,12 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11">
       <c r="A8" t="s">
         <v>159</v>
       </c>
       <c r="B8" s="22">
-        <v>43864</v>
+        <v>43893</v>
       </c>
       <c r="C8" s="19" t="s">
         <v>163</v>
@@ -5388,12 +5382,12 @@
         <v>450</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11">
       <c r="A9" t="s">
         <v>159</v>
       </c>
       <c r="B9" s="22">
-        <v>43865</v>
+        <v>43894</v>
       </c>
       <c r="C9" s="19" t="s">
         <v>163</v>
@@ -5423,12 +5417,12 @@
         <v>890</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11">
       <c r="A10" s="14" t="s">
         <v>182</v>
       </c>
       <c r="B10" s="22">
-        <v>43862</v>
+        <v>43891</v>
       </c>
       <c r="C10" s="19" t="s">
         <v>205</v>
@@ -5458,12 +5452,12 @@
         <v>100</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11">
       <c r="A11" s="14" t="s">
         <v>182</v>
       </c>
       <c r="B11" s="22">
-        <v>43863</v>
+        <v>43892</v>
       </c>
       <c r="C11" s="19" t="s">
         <v>205</v>
@@ -5493,12 +5487,12 @@
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11">
       <c r="A12" s="14" t="s">
         <v>182</v>
       </c>
       <c r="B12" s="22">
-        <v>43864</v>
+        <v>43893</v>
       </c>
       <c r="C12" s="19" t="s">
         <v>205</v>
@@ -5528,12 +5522,12 @@
         <v>450</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11">
       <c r="A13" s="14" t="s">
         <v>182</v>
       </c>
       <c r="B13" s="22">
-        <v>43865</v>
+        <v>43894</v>
       </c>
       <c r="C13" s="19" t="s">
         <v>205</v>
@@ -5563,12 +5557,12 @@
         <v>890</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11">
       <c r="A14" s="14" t="s">
         <v>181</v>
       </c>
       <c r="B14" s="22">
-        <v>43862</v>
+        <v>43891</v>
       </c>
       <c r="C14" s="19" t="s">
         <v>118</v>
@@ -5598,12 +5592,12 @@
         <v>100</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11">
       <c r="A15" s="14" t="s">
         <v>181</v>
       </c>
       <c r="B15" s="22">
-        <v>43863</v>
+        <v>43892</v>
       </c>
       <c r="C15" s="19" t="s">
         <v>118</v>
@@ -5633,12 +5627,12 @@
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11">
       <c r="A16" s="14" t="s">
         <v>181</v>
       </c>
       <c r="B16" s="22">
-        <v>43864</v>
+        <v>43893</v>
       </c>
       <c r="C16" s="19" t="s">
         <v>118</v>
@@ -5668,12 +5662,12 @@
         <v>450</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11">
       <c r="A17" s="14" t="s">
         <v>181</v>
       </c>
       <c r="B17" s="22">
-        <v>43865</v>
+        <v>43894</v>
       </c>
       <c r="C17" s="19" t="s">
         <v>118</v>
@@ -5703,12 +5697,12 @@
         <v>890</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11">
       <c r="A18" s="14" t="s">
         <v>158</v>
       </c>
       <c r="B18" s="22">
-        <v>43862</v>
+        <v>43891</v>
       </c>
       <c r="C18" s="19" t="s">
         <v>205</v>
@@ -5738,12 +5732,12 @@
         <v>100</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11">
       <c r="A19" s="14" t="s">
         <v>158</v>
       </c>
       <c r="B19" s="22">
-        <v>43863</v>
+        <v>43892</v>
       </c>
       <c r="C19" s="19" t="s">
         <v>205</v>
@@ -5773,12 +5767,12 @@
         <v>30</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11">
       <c r="A20" s="14" t="s">
         <v>158</v>
       </c>
       <c r="B20" s="22">
-        <v>43864</v>
+        <v>43893</v>
       </c>
       <c r="C20" s="19" t="s">
         <v>205</v>
@@ -5808,12 +5802,12 @@
         <v>450</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11">
       <c r="A21" s="14" t="s">
         <v>158</v>
       </c>
       <c r="B21" s="22">
-        <v>43865</v>
+        <v>43894</v>
       </c>
       <c r="C21" s="19" t="s">
         <v>205</v>
@@ -5849,16 +5843,16 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4">
       <c r="A1" s="4" t="s">
         <v>37</v>
       </c>
@@ -5872,12 +5866,12 @@
         <v>193</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4">
       <c r="A2" s="2" t="s">
         <v>49</v>
       </c>
       <c r="B2" s="24">
-        <v>43862</v>
+        <v>43891</v>
       </c>
       <c r="C2">
         <v>65</v>
@@ -5886,12 +5880,12 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4">
       <c r="A3" s="2" t="s">
         <v>49</v>
       </c>
       <c r="B3" s="24">
-        <v>43863</v>
+        <v>43892</v>
       </c>
       <c r="C3">
         <v>75</v>
@@ -5900,12 +5894,12 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4">
       <c r="A4" s="2" t="s">
         <v>49</v>
       </c>
       <c r="B4" s="24">
-        <v>43864</v>
+        <v>43893</v>
       </c>
       <c r="C4">
         <v>70</v>
@@ -5914,12 +5908,12 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4">
       <c r="A5" s="2" t="s">
         <v>49</v>
       </c>
       <c r="B5" s="24">
-        <v>43865</v>
+        <v>43894</v>
       </c>
       <c r="C5">
         <v>45</v>
@@ -5928,12 +5922,12 @@
         <v>55</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4">
       <c r="A6" s="2" t="s">
         <v>49</v>
       </c>
       <c r="B6" s="24">
-        <v>43866</v>
+        <v>43895</v>
       </c>
       <c r="C6">
         <v>25</v>
@@ -5942,12 +5936,12 @@
         <v>75</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4">
       <c r="A7" s="7" t="s">
         <v>159</v>
       </c>
-      <c r="B7" s="25">
-        <v>43862</v>
+      <c r="B7" s="24">
+        <v>43891</v>
       </c>
       <c r="C7">
         <v>50</v>
@@ -5956,12 +5950,12 @@
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4">
       <c r="A8" s="7" t="s">
         <v>159</v>
       </c>
-      <c r="B8" s="25">
-        <v>43863</v>
+      <c r="B8" s="24">
+        <v>43892</v>
       </c>
       <c r="C8">
         <v>55</v>
@@ -5970,12 +5964,12 @@
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4">
       <c r="A9" s="7" t="s">
         <v>159</v>
       </c>
-      <c r="B9" s="25">
-        <v>43864</v>
+      <c r="B9" s="24">
+        <v>43893</v>
       </c>
       <c r="C9">
         <v>60</v>
@@ -5984,12 +5978,12 @@
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4">
       <c r="A10" s="7" t="s">
         <v>159</v>
       </c>
-      <c r="B10" s="25">
-        <v>43865</v>
+      <c r="B10" s="24">
+        <v>43894</v>
       </c>
       <c r="C10">
         <v>65</v>
@@ -5998,12 +5992,12 @@
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4">
       <c r="A11" s="7" t="s">
         <v>159</v>
       </c>
-      <c r="B11" s="25">
-        <v>43866</v>
+      <c r="B11" s="24">
+        <v>43895</v>
       </c>
       <c r="C11">
         <v>70</v>
@@ -6012,12 +6006,12 @@
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4">
       <c r="A12" s="7" t="s">
         <v>181</v>
       </c>
-      <c r="B12" s="25">
-        <v>43862</v>
+      <c r="B12" s="24">
+        <v>43891</v>
       </c>
       <c r="C12">
         <v>30</v>
@@ -6026,12 +6020,12 @@
         <v>70</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4">
       <c r="A13" s="7" t="s">
         <v>181</v>
       </c>
-      <c r="B13" s="25">
-        <v>43863</v>
+      <c r="B13" s="24">
+        <v>43892</v>
       </c>
       <c r="C13">
         <v>70</v>
@@ -6040,12 +6034,12 @@
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4">
       <c r="A14" s="7" t="s">
         <v>181</v>
       </c>
-      <c r="B14" s="25">
-        <v>43864</v>
+      <c r="B14" s="24">
+        <v>43893</v>
       </c>
       <c r="C14">
         <v>65</v>
@@ -6054,12 +6048,12 @@
         <v>35</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4">
       <c r="A15" s="7" t="s">
         <v>181</v>
       </c>
-      <c r="B15" s="25">
-        <v>43865</v>
+      <c r="B15" s="24">
+        <v>43894</v>
       </c>
       <c r="C15">
         <v>55</v>
@@ -6068,12 +6062,12 @@
         <v>45</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4">
       <c r="A16" s="7" t="s">
         <v>181</v>
       </c>
-      <c r="B16" s="25">
-        <v>43866</v>
+      <c r="B16" s="24">
+        <v>43895</v>
       </c>
       <c r="C16">
         <v>50</v>
@@ -6082,12 +6076,12 @@
         <v>50</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4">
       <c r="A17" s="7" t="s">
         <v>181</v>
       </c>
       <c r="B17" s="25">
-        <v>43867</v>
+        <v>43896</v>
       </c>
       <c r="C17">
         <v>45</v>
@@ -6096,12 +6090,12 @@
         <v>55</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4">
       <c r="A18" s="14" t="s">
         <v>182</v>
       </c>
-      <c r="B18" s="26">
-        <v>43862</v>
+      <c r="B18" s="24">
+        <v>43891</v>
       </c>
       <c r="C18">
         <v>75</v>
@@ -6110,12 +6104,12 @@
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4">
       <c r="A19" s="14" t="s">
         <v>182</v>
       </c>
-      <c r="B19" s="26">
-        <v>43863</v>
+      <c r="B19" s="24">
+        <v>43892</v>
       </c>
       <c r="C19">
         <v>75</v>
@@ -6124,12 +6118,12 @@
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4">
       <c r="A20" s="14" t="s">
         <v>182</v>
       </c>
-      <c r="B20" s="26">
-        <v>43864</v>
+      <c r="B20" s="24">
+        <v>43893</v>
       </c>
       <c r="C20">
         <v>60</v>
@@ -6138,12 +6132,12 @@
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4">
       <c r="A21" s="14" t="s">
         <v>182</v>
       </c>
-      <c r="B21" s="26">
-        <v>43865</v>
+      <c r="B21" s="24">
+        <v>43894</v>
       </c>
       <c r="C21">
         <v>65</v>
@@ -6152,12 +6146,12 @@
         <v>35</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4">
       <c r="A22" s="14" t="s">
         <v>182</v>
       </c>
-      <c r="B22" s="26">
-        <v>43866</v>
+      <c r="B22" s="24">
+        <v>43895</v>
       </c>
       <c r="C22">
         <v>75</v>
@@ -6166,12 +6160,12 @@
         <v>25</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4">
       <c r="A23" s="14" t="s">
         <v>158</v>
       </c>
-      <c r="B23" s="26">
-        <v>43862</v>
+      <c r="B23" s="24">
+        <v>43891</v>
       </c>
       <c r="C23">
         <v>90</v>
@@ -6180,12 +6174,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4">
       <c r="A24" s="14" t="s">
         <v>158</v>
       </c>
-      <c r="B24" s="26">
-        <v>43863</v>
+      <c r="B24" s="24">
+        <v>43892</v>
       </c>
       <c r="C24">
         <v>80</v>
@@ -6194,12 +6188,12 @@
         <v>20</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4">
       <c r="A25" s="14" t="s">
         <v>158</v>
       </c>
-      <c r="B25" s="26">
-        <v>43864</v>
+      <c r="B25" s="24">
+        <v>43893</v>
       </c>
       <c r="C25">
         <v>75</v>
@@ -6208,12 +6202,12 @@
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4">
       <c r="A26" s="14" t="s">
         <v>158</v>
       </c>
-      <c r="B26" s="26">
-        <v>43865</v>
+      <c r="B26" s="24">
+        <v>43894</v>
       </c>
       <c r="C26">
         <v>65</v>
@@ -6222,12 +6216,12 @@
         <v>35</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4">
       <c r="A27" s="14" t="s">
         <v>158</v>
       </c>
-      <c r="B27" s="26">
-        <v>43866</v>
+      <c r="B27" s="24">
+        <v>43895</v>
       </c>
       <c r="C27">
         <v>70</v>

</xml_diff>